<commit_message>
cracion de primer tabla
</commit_message>
<xml_diff>
--- a/notebooks/pivot_table.xlsx
+++ b/notebooks/pivot_table.xlsx
@@ -7,37 +7,31 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabla Código de Cierre" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
-  <si>
-    <t>mes_cierre</t>
-  </si>
-  <si>
-    <t>sin_corregir</t>
-  </si>
-  <si>
-    <t>Diciembre</t>
-  </si>
-  <si>
-    <t>Enero</t>
-  </si>
-  <si>
-    <t>Febrero</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+  <si>
+    <t>Código de Cierre</t>
+  </si>
+  <si>
+    <t>Sin Reclasificar</t>
   </si>
   <si>
     <t>TOTAL</t>
   </si>
   <si>
-    <t>Sin corregir</t>
-  </si>
-  <si>
-    <t>Código de cierre</t>
+    <t>DIC</t>
+  </si>
+  <si>
+    <t>ENE</t>
+  </si>
+  <si>
+    <t>FEB</t>
   </si>
   <si>
     <t>ACI</t>
@@ -419,89 +413,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="1.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
+      <c r="F2" s="1"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="s">
+      <c r="C5">
+        <v>41</v>
+      </c>
+      <c r="D5">
+        <v>26</v>
+      </c>
+      <c r="E5">
+        <v>19</v>
+      </c>
+      <c r="F5">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
         <v>8</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="E4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>41</v>
-      </c>
-      <c r="C5">
-        <v>26</v>
-      </c>
-      <c r="D5">
-        <v>19</v>
-      </c>
-      <c r="E5">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -512,110 +506,134 @@
       <c r="E6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7">
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
         <v>41</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>19</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>3</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8">
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
         <v>17</v>
-      </c>
-      <c r="C8">
-        <v>9</v>
       </c>
       <c r="D8">
         <v>9</v>
       </c>
       <c r="E8">
+        <v>9</v>
+      </c>
+      <c r="F8">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:6">
+      <c r="A9" s="1">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>104</v>
+      </c>
+      <c r="D10">
+        <v>59</v>
+      </c>
+      <c r="E10">
+        <v>36</v>
+      </c>
+      <c r="F10">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="B9">
+      <c r="C11">
+        <v>163</v>
+      </c>
+      <c r="D11">
+        <v>124</v>
+      </c>
+      <c r="E11">
+        <v>107</v>
+      </c>
+      <c r="F11">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
         <v>2</v>
       </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10">
-        <v>104</v>
-      </c>
-      <c r="C10">
-        <v>59</v>
-      </c>
-      <c r="D10">
-        <v>36</v>
-      </c>
-      <c r="E10">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11">
-        <v>163</v>
-      </c>
-      <c r="C11">
-        <v>124</v>
-      </c>
-      <c r="D11">
-        <v>107</v>
-      </c>
-      <c r="E11">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12">
+      <c r="C12">
         <v>267</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>183</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>143</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>593</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>